<commit_message>
Ajustes en script.js para primer entrega proyecto
</commit_message>
<xml_diff>
--- a/media/Inventario asegurables.xlsx
+++ b/media/Inventario asegurables.xlsx
@@ -205,6 +205,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -218,15 +227,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,18 +554,18 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -763,18 +763,18 @@
         <v>10</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -987,18 +987,18 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
@@ -1196,18 +1196,18 @@
         <v>5</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="16" t="s">
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">

</xml_diff>

<commit_message>
adjustments to ajax function
</commit_message>
<xml_diff>
--- a/media/Inventario asegurables.xlsx
+++ b/media/Inventario asegurables.xlsx
@@ -16,20 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Nave</t>
   </si>
   <si>
-    <t>Dreadnought Super Star Destroyer</t>
-  </si>
-  <si>
     <t>Star Destroyer</t>
   </si>
   <si>
-    <t>Corellian Corvette</t>
-  </si>
-  <si>
     <t>Corellian Freighter</t>
   </si>
   <si>
@@ -73,6 +67,21 @@
   </si>
   <si>
     <t>Prima Anual</t>
+  </si>
+  <si>
+    <t>Executor Class Star Dreadnought</t>
+  </si>
+  <si>
+    <t>https://swapi.dev/api/starships/</t>
+  </si>
+  <si>
+    <t>CR90 Corellian Corvette</t>
+  </si>
+  <si>
+    <t>BTL Y-wing</t>
+  </si>
+  <si>
+    <t>T-65 X-wing</t>
   </si>
 </sst>
 </file>
@@ -115,12 +124,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -151,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -164,14 +179,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -474,11 +491,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -500,49 +515,51 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="G1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="13"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="K2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -550,54 +567,54 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="11">
+        <v>15</v>
+      </c>
+      <c r="G3" s="10">
         <v>0.5</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>0.65</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>0.85</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>1</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>0.5</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>0.65</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>0.85</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4">
         <v>150000000</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6">
         <v>0.1</v>
@@ -642,64 +659,64 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4">
-        <v>325000000000</v>
+        <v>1143350000</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="6">
         <v>0.1</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ref="E5:E9" si="2">100/10</f>
+        <f t="shared" ref="E5:E12" si="2">100/10</f>
         <v>10</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="4">
         <f>($B$5-($B$5*$D$5*$F$5))*G3</f>
-        <v>162500000000</v>
+        <v>571675000</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" ref="H5:J5" si="3">($B$5-($B$5*$D$5*$F$5))*H3</f>
-        <v>211250000000</v>
+        <v>743177500</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="3"/>
-        <v>276250000000</v>
+        <v>971847500</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="3"/>
-        <v>325000000000</v>
+        <v>1143350000</v>
       </c>
       <c r="K5" s="4">
         <f>(G5/$E$5)*(G3/$E$5)</f>
-        <v>812500000</v>
+        <v>2858375</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" ref="L5:N5" si="4">(H5/$E$5)*(H3/$E$5)</f>
-        <v>1373125000</v>
+        <v>4830653.75</v>
       </c>
       <c r="M5" s="4">
         <f t="shared" si="4"/>
-        <v>2348125000</v>
+        <v>8260703.7499999991</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" si="4"/>
-        <v>3250000000</v>
+        <v>11433500</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
+      <c r="A6" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>88000000</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="6">
         <v>0.1</v>
@@ -744,13 +761,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4">
         <v>3500000</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="6">
         <v>0.1</v>
@@ -794,14 +811,14 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
+      <c r="A8" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="B8" s="4">
         <v>1500000</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="6">
         <v>0.1</v>
@@ -846,13 +863,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="4">
         <v>100000</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="6">
         <v>0.1</v>
@@ -893,6 +910,108 @@
       <c r="N9" s="4">
         <f>(J9/$E$9)*(J3/$E$9)</f>
         <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4">
+        <v>134999</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="4">
+        <f>($B$11-($B$11*$D$11*$F$11))*G3</f>
+        <v>67499.5</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" ref="H11:J11" si="5">($B$11-($B$11*$D$11*$F$11))*H3</f>
+        <v>87749.35</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="5"/>
+        <v>114749.15</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="5"/>
+        <v>134999</v>
+      </c>
+      <c r="K11" s="4">
+        <f>(G11/$E$11)*(G3/$E$11)</f>
+        <v>337.4975</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" ref="L11:N11" si="6">(H11/$E$11)*(H3/$E$11)</f>
+        <v>570.37077500000009</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="6"/>
+        <v>975.36777499999982</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="6"/>
+        <v>1349.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4">
+        <v>149999</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="4">
+        <f>($B$12-($B$12*$D$12*$F$12))*G3</f>
+        <v>74999.5</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" ref="H12:J12" si="7">($B$12-($B$12*$D$12*$F$12))*H3</f>
+        <v>97499.35</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="7"/>
+        <v>127499.15</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="7"/>
+        <v>149999</v>
+      </c>
+      <c r="K12" s="4">
+        <f>(G12/$E$12)*(G3/$E$12)</f>
+        <v>374.9975</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" ref="L12:N12" si="8">(H12/$E$12)*(H3/$E$12)</f>
+        <v>633.74577500000009</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="8"/>
+        <v>1083.7427749999997</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="8"/>
+        <v>1499.99</v>
       </c>
     </row>
   </sheetData>
@@ -907,9 +1026,12 @@
     <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5"/>
     <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="A2" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="C12" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>